<commit_message>
TimeSheet Week3 of summer practice
</commit_message>
<xml_diff>
--- a/Timesheet_Radu_STANA.xlsx
+++ b/Timesheet_Radu_STANA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\Convertor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBF079A-59E7-4D1E-87AE-5DACFA7CDDD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D739FD0-D967-4020-9696-CCAD4B5A1B23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Hours Worked</t>
   </si>
@@ -92,6 +92,21 @@
   </si>
   <si>
     <t>Documentation</t>
+  </si>
+  <si>
+    <t>Meetings &amp; Documentation CANoe + Capl</t>
+  </si>
+  <si>
+    <t>Documentation CANoe</t>
+  </si>
+  <si>
+    <t>Meeting &amp; Documentation CANoe</t>
+  </si>
+  <si>
+    <t>Meeting + Project Develop</t>
+  </si>
+  <si>
+    <t>Project Develop</t>
   </si>
 </sst>
 </file>
@@ -755,7 +770,7 @@
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -810,11 +825,11 @@
     <row r="5" spans="2:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="15">
         <f>SUM(TimeSheet[Hours Worked])</f>
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C5" s="16">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -994,57 +1009,81 @@
       <c r="B15" s="9">
         <v>44026</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="5">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="F15" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G15" s="4">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Pause End]]+TimeSheet[[#This Row],[Pause Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="9">
         <v>44027</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="5">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="F16" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G16" s="4">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Pause End]]+TimeSheet[[#This Row],[Pause Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="9">
         <v>44028</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="5">
+        <v>0.375</v>
+      </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="F17" s="5">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="G17" s="4">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Pause End]]+TimeSheet[[#This Row],[Pause Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="5"/>
+        <v>3.9999999999999991</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="9">
         <v>44029</v>
       </c>
-      <c r="C18" s="5"/>
+      <c r="C18" s="5">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="F18" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G18" s="4">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Pause End]]+TimeSheet[[#This Row],[Pause Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H18" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="10">
@@ -1078,43 +1117,61 @@
       <c r="B21" s="9">
         <v>44032</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="5">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
+      <c r="F21" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G21" s="4">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Pause End]]+TimeSheet[[#This Row],[Pause Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="9">
         <v>44033</v>
       </c>
-      <c r="C22" s="5"/>
+      <c r="C22" s="5">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
+      <c r="F22" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G22" s="4">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Pause End]]+TimeSheet[[#This Row],[Pause Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="9">
         <v>44034</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C23" s="5">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+      <c r="F23" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G23" s="4">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Pause End]]+TimeSheet[[#This Row],[Pause Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="9">
@@ -2098,7 +2155,7 @@
     </row>
   </sheetData>
   <dataValidations count="23">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:E1 D3:E3 A2:A1048576 H7:H93 I6:XFD93 H94:XFD1048576 F1:XFD5 B7:G1048576" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:E1 D3:E3 A2:A1048576 B7:G1048576 I6:XFD93 H94:XFD1048576 F1:XFD5 H7:H93" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Use this worksheet to track hours worked in a work week. Enter Date and Times in TimeSheet table. Total Hours, Regular Hours and Overtime Hours are automatically calculated" sqref="A1" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell.  Enter Employee and Manager details in cells below" sqref="B1" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Employee Name, Email and Phone in cells at right" sqref="B2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
@@ -2135,21 +2192,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F3FD9086AB4B47439E87CD25B1636040" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="19b9817df20194a8bdc05a525b7bfb11">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eb3464dd-34a5-4bf8-acc6-8c7fb799d1f1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1474b9b216da049053a6b591099c35f0" ns2:_="">
     <xsd:import namespace="eb3464dd-34a5-4bf8-acc6-8c7fb799d1f1"/>
@@ -2281,31 +2323,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69B3D4F9-5C67-4FD7-9808-0F1379841A00}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="eb3464dd-34a5-4bf8-acc6-8c7fb799d1f1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6707A839-5E5E-450C-8A08-8F1108526EA7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC4AA2FD-F1E9-49AE-9781-86B62BD0B84E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2321,4 +2354,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6707A839-5E5E-450C-8A08-8F1108526EA7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69B3D4F9-5C67-4FD7-9808-0F1379841A00}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="eb3464dd-34a5-4bf8-acc6-8c7fb799d1f1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Time sheet for Week7
</commit_message>
<xml_diff>
--- a/Timesheet_Radu_STANA.xlsx
+++ b/Timesheet_Radu_STANA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\Convertor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22D43CD-650D-45AE-A93F-F215669DDD1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D065AE0E-E5BC-434B-B078-8868C92A4C15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
     <t>Hours Worked</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>Project Develop + HR Meeting</t>
+  </si>
+  <si>
+    <t>Project Develop + Meetings</t>
   </si>
 </sst>
 </file>
@@ -767,10 +770,10 @@
   <dimension ref="B1:H93"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="C44" sqref="C44"/>
+      <selection pane="bottomRight" activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -825,11 +828,11 @@
     <row r="5" spans="2:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="15">
         <f>SUM(TimeSheet[Hours Worked])</f>
-        <v>118</v>
+        <v>148</v>
       </c>
       <c r="C5" s="16">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>118</v>
+        <v>148</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -1555,29 +1558,41 @@
       <c r="B45" s="9">
         <v>44056</v>
       </c>
-      <c r="C45" s="5"/>
+      <c r="C45" s="5">
+        <v>0.375</v>
+      </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
+      <c r="F45" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G45" s="4">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Pause End]]+TimeSheet[[#This Row],[Pause Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H45" s="5"/>
+        <v>5.0000000000000009</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="46" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="9">
         <v>44057</v>
       </c>
-      <c r="C46" s="5"/>
+      <c r="C46" s="5">
+        <v>0.375</v>
+      </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
+      <c r="F46" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G46" s="4">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Pause End]]+TimeSheet[[#This Row],[Pause Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H46" s="5"/>
+        <v>5.0000000000000009</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="47" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="10">
@@ -1611,57 +1626,81 @@
       <c r="B49" s="9">
         <v>44060</v>
       </c>
-      <c r="C49" s="5"/>
+      <c r="C49" s="5">
+        <v>0.375</v>
+      </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
+      <c r="F49" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G49" s="4">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Pause End]]+TimeSheet[[#This Row],[Pause Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H49" s="5"/>
+        <v>5.0000000000000009</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="50" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="9">
         <v>44061</v>
       </c>
-      <c r="C50" s="5"/>
+      <c r="C50" s="5">
+        <v>0.375</v>
+      </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
+      <c r="F50" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G50" s="4">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Pause End]]+TimeSheet[[#This Row],[Pause Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H50" s="5"/>
+        <v>5.0000000000000009</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="51" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="9">
         <v>44062</v>
       </c>
-      <c r="C51" s="5"/>
+      <c r="C51" s="5">
+        <v>0.375</v>
+      </c>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
+      <c r="F51" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G51" s="4">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Pause End]]+TimeSheet[[#This Row],[Pause Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H51" s="5"/>
+        <v>5.0000000000000009</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="52" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="9">
         <v>44063</v>
       </c>
-      <c r="C52" s="5"/>
+      <c r="C52" s="5">
+        <v>0.375</v>
+      </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
+      <c r="F52" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G52" s="4">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Pause End]]+TimeSheet[[#This Row],[Pause Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H52" s="5"/>
+        <v>5.0000000000000009</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="53" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="9">
@@ -2239,7 +2278,7 @@
     </row>
   </sheetData>
   <dataValidations count="23">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:E1 D3:E3 A2:A1048576 H7:H93 I6:XFD93 H94:XFD1048576 F1:XFD5 B7:G1048576" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:E1 D3:E3 A2:A1048576 B7:G1048576 I6:XFD93 H94:XFD1048576 F1:XFD5 H7:H93" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Use this worksheet to track hours worked in a work week. Enter Date and Times in TimeSheet table. Total Hours, Regular Hours and Overtime Hours are automatically calculated" sqref="A1" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell.  Enter Employee and Manager details in cells below" sqref="B1" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Employee Name, Email and Phone in cells at right" sqref="B2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
@@ -2276,21 +2315,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F3FD9086AB4B47439E87CD25B1636040" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="19b9817df20194a8bdc05a525b7bfb11">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eb3464dd-34a5-4bf8-acc6-8c7fb799d1f1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1474b9b216da049053a6b591099c35f0" ns2:_="">
     <xsd:import namespace="eb3464dd-34a5-4bf8-acc6-8c7fb799d1f1"/>
@@ -2422,31 +2446,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69B3D4F9-5C67-4FD7-9808-0F1379841A00}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="eb3464dd-34a5-4bf8-acc6-8c7fb799d1f1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6707A839-5E5E-450C-8A08-8F1108526EA7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC4AA2FD-F1E9-49AE-9781-86B62BD0B84E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2462,4 +2477,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6707A839-5E5E-450C-8A08-8F1108526EA7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69B3D4F9-5C67-4FD7-9808-0F1379841A00}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="eb3464dd-34a5-4bf8-acc6-8c7fb799d1f1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Timesheet for week 9
</commit_message>
<xml_diff>
--- a/Timesheet_Radu_STANA.xlsx
+++ b/Timesheet_Radu_STANA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\Convertor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D065AE0E-E5BC-434B-B078-8868C92A4C15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E25CC8-E8A4-4109-ADC5-A1351742FFCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
   <si>
     <t>Hours Worked</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Project Develop + Meetings</t>
+  </si>
+  <si>
+    <t>Research</t>
   </si>
 </sst>
 </file>
@@ -770,10 +773,10 @@
   <dimension ref="B1:H93"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B112" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E57" sqref="E57"/>
+      <selection pane="bottomRight" activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -828,11 +831,11 @@
     <row r="5" spans="2:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="15">
         <f>SUM(TimeSheet[Hours Worked])</f>
-        <v>148</v>
+        <v>180</v>
       </c>
       <c r="C5" s="16">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>148</v>
+        <v>180</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -1706,15 +1709,21 @@
       <c r="B53" s="9">
         <v>44064</v>
       </c>
-      <c r="C53" s="5"/>
+      <c r="C53" s="5">
+        <v>0.375</v>
+      </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
+      <c r="F53" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G53" s="4">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Pause End]]+TimeSheet[[#This Row],[Pause Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H53" s="5"/>
+        <v>5.0000000000000009</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="54" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="10">
@@ -1748,29 +1757,41 @@
       <c r="B56" s="9">
         <v>44067</v>
       </c>
-      <c r="C56" s="5"/>
+      <c r="C56" s="5">
+        <v>0.375</v>
+      </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
+      <c r="F56" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G56" s="4">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Pause End]]+TimeSheet[[#This Row],[Pause Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H56" s="5"/>
+        <v>5.0000000000000009</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="57" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="9">
         <v>44068</v>
       </c>
-      <c r="C57" s="5"/>
+      <c r="C57" s="5">
+        <v>0.375</v>
+      </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
+      <c r="F57" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G57" s="4">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Pause End]]+TimeSheet[[#This Row],[Pause Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H57" s="5"/>
+        <v>5.0000000000000009</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="58" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="9">
@@ -1874,43 +1895,61 @@
       <c r="B65" s="9">
         <v>44076</v>
       </c>
-      <c r="C65" s="5"/>
+      <c r="C65" s="5">
+        <v>0.375</v>
+      </c>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
+      <c r="F65" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G65" s="4">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Pause End]]+TimeSheet[[#This Row],[Pause Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H65" s="5"/>
+        <v>5.0000000000000009</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="66" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="9">
         <v>44077</v>
       </c>
-      <c r="C66" s="5"/>
+      <c r="C66" s="5">
+        <v>0.375</v>
+      </c>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
+      <c r="F66" s="5">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="G66" s="4">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Pause End]]+TimeSheet[[#This Row],[Pause Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H66" s="5"/>
+        <v>6.9999999999999991</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="67" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="9">
         <v>44078</v>
       </c>
-      <c r="C67" s="5"/>
+      <c r="C67" s="5">
+        <v>0.375</v>
+      </c>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
+      <c r="F67" s="5">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G67" s="4">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Pause End]]+TimeSheet[[#This Row],[Pause Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H67" s="5"/>
+        <v>5.0000000000000009</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="68" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="10">
@@ -2315,6 +2354,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F3FD9086AB4B47439E87CD25B1636040" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="19b9817df20194a8bdc05a525b7bfb11">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eb3464dd-34a5-4bf8-acc6-8c7fb799d1f1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1474b9b216da049053a6b591099c35f0" ns2:_="">
     <xsd:import namespace="eb3464dd-34a5-4bf8-acc6-8c7fb799d1f1"/>
@@ -2446,22 +2500,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69B3D4F9-5C67-4FD7-9808-0F1379841A00}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="eb3464dd-34a5-4bf8-acc6-8c7fb799d1f1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6707A839-5E5E-450C-8A08-8F1108526EA7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC4AA2FD-F1E9-49AE-9781-86B62BD0B84E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2477,28 +2540,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6707A839-5E5E-450C-8A08-8F1108526EA7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69B3D4F9-5C67-4FD7-9808-0F1379841A00}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="eb3464dd-34a5-4bf8-acc6-8c7fb799d1f1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>